<commit_message>
Update deploy doc for v5.4.130716
</commit_message>
<xml_diff>
--- a/10_Sony_Select_Service/Deploy/v5.4.130716/Deploy Steps/Deployment Steps.xlsx
+++ b/10_Sony_Select_Service/Deploy/v5.4.130716/Deploy Steps/Deployment Steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="更新步骤" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>PlayNow库</t>
   </si>
@@ -101,9 +101,6 @@
     </r>
   </si>
   <si>
-    <t>删除D:\PlaynowService目录下除AppSettings和Web.config的所有文件</t>
-  </si>
-  <si>
     <t>更新PlayNow Windows Service</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>USE [PlayNow]
 INSERT INTO dbo.PN_Module (MenuId, ModuleName, ModulePath) VALUES ('3','页面调用统计','Statistic/ExternalAccess.aspx')
 GO</t>
-  </si>
-  <si>
-    <t>在表PN_Module上点击右键, 选择编辑前200行，找到‘ModuleName’等于‘页面调用统计’行，然后右键，选择删除</t>
   </si>
   <si>
     <t>表PN_AdInfo添加</t>
@@ -206,15 +200,281 @@
     <t>在存储过程SP_ExternalAccessStatistic上点击右键, 选择删除</t>
   </si>
   <si>
-    <t>不用处理</t>
-  </si>
-  <si>
     <t>更新存储过程SP_MessageStatistic</t>
   </si>
   <si>
-    <t xml:space="preserve">USE [PlayNowLog]
-GO
-/****** Object:  StoredProcedure [dbo].[SP_MessageStatistic]    Script Date: 07/08/2013 11:46:34 ******/
+    <t>更新存储过程SP_DownSourceStatistic</t>
+  </si>
+  <si>
+    <t>更新存储过程SP_DeleteStatistic</t>
+  </si>
+  <si>
+    <t>USE [PlayNowLog]
+GO
+/****** Object:  Table [dbo].[PN_S_ExternalAccess]    Script Date: 05/10/2013 10:23:48 ******/
+SET ANSI_NULLS ON
+GO
+SET QUOTED_IDENTIFIER ON
+GO
+CREATE TABLE [dbo].[PN_S_ExternalAccess](
+                [Id] [int] IDENTITY(1,1) NOT NULL,
+                [Name] [nvarchar](200) NULL,
+                [Alias] [nvarchar](200) NULL,
+                [AccessCount] [int] NULL,
+                [CreateTime] [datetime] NULL,
+                [MachineType] [nvarchar](50) NULL,
+CONSTRAINT [PK_PN_ZONE] PRIMARY KEY CLUSTERED 
+(
+                [Id] ASC
+)WITH (PAD_INDEX  = OFF, STATISTICS_NORECOMPUTE  = OFF, IGNORE_DUP_KEY = OFF, ALLOW_ROW_LOCKS  = ON, ALLOW_PAGE_LOCKS  = ON) ON [PRIMARY]
+) ON [PRIMARY]
+GO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">修改D:\PlaynowService\AppSettings目录下AppSettings.xml文件：
+ 在该文件中
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“&lt;appSettings&gt;”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                后面添加如下内容：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">       &lt;!-- 日志分析器  name：分析器名字， state：分析器状态，on：是可用，off：不可用,
+       platform:平台类型（web/phone/tv）, machineTypes:机器类型，version：客户端版本--&gt;
+  &lt;LogAnalyzers&gt;
+    &lt;LogAnalyzer name="GoogleAnalytics" state="on" platform="phone" machineTypes="" version=""/&gt;
+    &lt;!--&lt;LogAnalyzer name="PlayNowAnalytics" state="off" platform="" machineTypes="" version=""/&gt;--&gt;
+  &lt;/LogAnalyzers&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <t>更新WebAppStore</t>
+  </si>
+  <si>
+    <t>在windows service中启动playnowlogimport服务</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">修改D:\PlayNowWS_LogImport\WinService目录下PlayNowService.WinServices.exe.config文件：
+ 在该文件中
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“&lt;appSettings&gt;”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                后面添加如下内容：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      &lt;!--download更新每次提交记录数--&gt;
+      &lt;add key="DownloadCommitCount" value="3000" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>执行如下命令
+cd C:\WINDOWS\Microsoft.NET\Framework\v4.0.30319
+installutil.exe D:\PlayNowWS_LogImport\WinService\PlayNowService.WinService.Log.exe</t>
+  </si>
+  <si>
+    <t>删除D:\WebAppStore目录下除Web.config的所有文件</t>
+  </si>
+  <si>
+    <t>删除D:\PlayNowManage目录下除Web.config的所有文件</t>
+  </si>
+  <si>
+    <t>所有安装包所在文件夹为v5.4.130716\Deploy Packages\PlayNowService</t>
+  </si>
+  <si>
+    <t>复制文件夹v5.4.130716\Deploy Packages\PlayNowService下的全部文件到D:\PlaynowService目录</t>
+  </si>
+  <si>
+    <t>所有安装包所在文件夹为v5.4.130716\Deploy Packages\WinService</t>
+  </si>
+  <si>
+    <t>将更新文件夹v5.4.130716\Deploy Packages\WinService下的内容拷贝到D:\PlayNowWS_LogImport\WinService目录下</t>
+  </si>
+  <si>
+    <t>所有安装包所在文件夹为 v5.4.130716\Deploy Packages\PlayNowManager</t>
+  </si>
+  <si>
+    <t>复制文件夹 v5.4.130716\Deploy Packages\PlayNowManager下的全部文件到D:\PlayNowManage 目录</t>
+  </si>
+  <si>
+    <t>所有安装包所在文件夹为  v5.4.130716\Deploy Packages\WebAppStore</t>
+  </si>
+  <si>
+    <t>复制文件夹v5.4.130716\Deploy Packages\WebAppStore下的全部文件到D:\WebAppStore目录</t>
+  </si>
+  <si>
+    <t>USE [PlayNowLog]
+GO
+/****** 对象:  StoredProcedure [dbo].[SP_ClinetPVStatistic]    脚本日期: 01/07/2014 22:38:57 ******/
+SET ANSI_NULLS ON
+GO
+SET QUOTED_IDENTIFIER ON
+GO
+-- =============================================
+-- Author:  &lt;Author,,Name&gt;
+-- Create date: &lt;Create Date,,&gt;
+-- Description: Clinet-Pv  分析 包括PlayNow, 百度，其中在做分析插入之前要做一次删除
+-- =============================================
+ALTER PROCEDURE [dbo].[SP_ClinetPVStatistic] 
+ -- Add the parameters for the stored procedure here
+ @BeginTime Datetime, 
+ @EndTime Datetime
+AS
+BEGIN
+ -- SET NOCOUNT ON added to prevent extra result sets from
+ -- interfering with SELECT statements.
+ SET NOCOUNT ON;
+--2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
+-- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
+--declare @errorCount int=0 --错误的累加
+declare @errorCount int 
+set @errorCount=0 
+begin  tran --开始事务
+--declare @BeginTime datetime
+--declare @EndTime datetime
+set @BeginTime= cast( convert(varchar(10),@BeginTime,120)as datetime)-- CAST(@BeginTime as datetime) --开始时间
+set @EndTime= cast( convert(varchar(10),DATEADD(DD,1, CAST(@EndTime as datetime)),120)as datetime) --DATEADD(DD,1, CAST(@EndTime as datetime)) --结束时间
+-- 分析前先删除 某一时间段的数据
+delete from  dbo.PN_S_ClinetPV where CreateTime&gt;=@BeginTime and  CreateTime&lt;@EndTime
+-- PlayNow Client-pv 分析
+insert into dbo.PN_S_ClinetPV(
+  Home, WidgetToHome, AppDetail, WidgetToAppDetail, AppComment,
+  AppRelate, Search, SearchResult, Recommend, RankApp, RankGame,
+  Zone, WidgetToZone, ZoneDetail, WidgetToZoneDetail, CategoryApp, 
+  CategoryGame, CategoryDetail, WapDownload, WidgetToAppRank,
+  WidgetToGameRank, ContentOrigin, MachineType, NewApp,NewGame,CreateTime
+)
+SELECT 
+SUM(CASE WHEN (IntentFromId!='1' or  IntentFromId is null) and pageName='首页' THEN 1 ELSE 0 END) 首页,
+SUM(CASE WHEN IntentFromId='1' AND pageName='首页' THEN 1 ELSE 0 END) 由Widget进入首页,
+SUM(CASE WHEN  (IntentFromId!='1' or  IntentFromId is null) and pageName='应用详情' THEN 1 ELSE 0 END) 应用详情, 
+SUM(CASE WHEN IntentFromId='1' AND pageName='应用详情' THEN 1 ELSE 0 END) 由Widget进入应用详情,
+sum(CASE pageName WHEN '应用评论'     THEN 1 else 0 end) 应用评论, 
+sum(CASE pageName WHEN '应用相关'     THEN 1 else 0 end) 应用相关, 
+sum(CASE pageName WHEN '搜索'     THEN 1 else 0 end) 搜索,
+sum(CASE pageName WHEN '搜索结果'     THEN 1 else 0 end) 搜索结果,
+sum(CASE pageName WHEN '推荐'     THEN 1 else 0 end) 推荐, 
+sum(CASE  WHEN (IntentFromId!='1' or  IntentFromId is null) and  pageName='排行应用'     THEN 1 else 0 end) 排行应用,
+sum(CASE  WHEN (IntentFromId!='1' or  IntentFromId is null) and  pageName='排行游戏'  THEN 1 else 0 end) 排行游戏,
+SUM(CASE WHEN (IntentFromId!='1' or  IntentFromId is null) and pageName='专区' THEN 1 ELSE 0 END) 专区, 
+SUM(CASE WHEN IntentFromId='1' AND pageName='专区' THEN 1 ELSE 0 END) 由Widget进入专区,
+SUM(CASE WHEN (IntentFromId!='1' or  IntentFromId is null) and pageName='专区详情' THEN 1 ELSE 0 END) 专区详情, 
+SUM(CASE WHEN IntentFromId='1' AND pageName='专区详情' THEN 1 ELSE 0 END) 由Widget进入专区详情,
+sum(CASE pageName WHEN '分类应用'     THEN 1 else 0 end) 分类应用, 
+sum(CASE pageName WHEN '分类游戏'     THEN 1 else 0 end) 分类游戏, 
+sum(CASE pageName WHEN '分类详情'     THEN 1 else 0 end) 分类详情,
+sum(CASE pageName WHEN 'Wap下载'     THEN 1 else 0 end) Wap下载 ,
+sum(CASE  WHEN IntentFromId='1' And pageName ='排行应用'     THEN 1 else 0 end) 由widget进入应用排行,
+sum(CASE  WHEN IntentFromId='1' And pageName ='排行游戏'     THEN 1 else 0 end) 由widget进入游戏排行,
+'PlayNow',
+MachineType,
+sum(CASE pageName WHEN '新品应用'     THEN 1 else 0 end) 新品应用, 
+sum(CASE pageName WHEN '新品游戏'     THEN 1 else 0 end) 新品游戏, 
+--cast(DateTime as date )
+cast( convert(varchar(10),DateTime,120)as datetime)
+from dbo.PN_Log_PageViewInfo 
+where (IntentFromId !=3 or IntentFromId is null) and  DateTime&gt;=@BeginTime and  DateTime&lt;@EndTime
+--and PageName in('首页','应用详情','应用评论','应用相关','搜索','搜索结果', '推荐','排行应用','排行游戏',
+--'专区','专区详情','分类应用','分类游戏','分类详情' ,'Wap下载')
+-- Group by cast(DateTime as date ),MachineType
+Group by cast( convert(varchar(10),DateTime,120)as datetime),MachineType
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+--百度Clinet-PV 分析
+insert into dbo.PN_S_ClinetPV(
+ Home, WidgetToHome,  WidgetToAppDetail, AppComment,
+  AppRelate, Search, Recommend, RankApp, RankGame,
+  Zone, WidgetToZone, ZoneDetail, WidgetToZoneDetail, CategoryApp, 
+  CategoryGame, CategoryDetail, WapDownload, WidgetToAppRank,
+  WidgetToGameRank,NewApp,NewGame,
+  AppDetail,  SearchResult,ContentOrigin, MachineType, CreateTime
+)
+SELECT 
+ 0,0,0,0,
+ 0,0,0,0,
+ 0,0,0,0,
+ 0,0,0,0,
+ 0,0,0,0,0,
+SUM(CASE WHEN pageName='应用详情' THEN 1 ELSE 0 END) 应用详情, 
+sum(CASE pageName WHEN '搜索结果'     THEN 1 else 0 end) 搜索结果,
+'百度', 
+MachineType,
+--cast(DateTime as date )
+cast( convert(varchar(10),DateTime,120)as datetime)
+from dbo.PN_Log_PageViewInfo 
+where IntentFromId =3  and  DateTime&gt;=@BeginTime and  DateTime&lt;@EndTime
+and PageName in('应用详情','搜索结果')
+--Group by cast(DateTime as date ),MachineType
+Group by cast( convert(varchar(10),DateTime,120)as datetime),MachineType
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+if(@errorCount&gt;0)
+ begin
+  rollback --如果有错，就回滚事务
+ end
+else
+ begin
+  commit tran --如果没有错，就提交事务
+ end
+END
+GO</t>
+  </si>
+  <si>
+    <t>USE [PlayNowLog]
+GO
+/****** Object:  StoredProcedure [dbo].[SP_MessageStatistic]    Script Date: 07/09/2013 15:36:07 ******/
 SET ANSI_NULLS ON
 GO
 SET QUOTED_IDENTIFIER ON
@@ -236,7 +496,6 @@
 --declare @errorCount int=0 --错误的累加
 --2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
 -- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
---2013/7/4 jiaoxuhuan ,添加machineType过滤条件。
 declare @errorCount int 
 set @errorCount=0 
 begin  tran --开始事务
@@ -257,27 +516,20 @@
     select COUNT(*) from [PN_Log_Message] as A 
      where C.MessageId=A.MessageId and IsValid=1 and   
     --CAST(A.CreateTime as date)=cast(C.CreateTime as date) ) as GetCount, 
-    cast( convert(varchar(10),A.CreateTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime)
-    and A.MachineType=C.MachineType
-     ) as GetCount, 
+    cast( convert(varchar(10),A.CreateTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) ) as GetCount, 
     (select COUNT(*) from [PN_Log_PageViewInfo] as B 
     where C.MessageId=B.ContentId AND IntentFromId=4 and
     -- CAST(B.DateTime as date)=cast(C.CreateTime as date) ) as PVCount,
-    cast( convert(varchar(10),B.DateTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) 
-    and B.MachineType=C.MachineType
-    )as PVCount,
+    cast( convert(varchar(10),B.DateTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) )as PVCount,
     (
     select COUNT(*) from [PN_Order] as D 
     where C.MessageId=D.ContentId and IntentFromId=4 and
      --CAST(D.StartTime as date)=cast(C.CreateTime as date) ) as DownCount,
-     cast( convert(varchar(10),D.StartTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) 
-      and D.MachineType=C.MachineType
-     )as DownCount,
+     cast( convert(varchar(10),D.StartTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) )as DownCount,
      (select COUNT(*) from [PN_Order] as G 
        where C.MessageId=G.ContentId and IntentFromId=4 and
       -- CAST(G.StartTime as date)=cast(C.CreateTime as date)  
      cast( convert(varchar(10),G.StartTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime)
-     and G.MachineType=C.MachineType
        and EndTime is not null) as DownCompleteCount
     --,CAST(CreateTime as date) dTime
     ,cast( convert(varchar(10),CreateTime,120)as datetime) dTime
@@ -297,13 +549,216 @@
   commit tran --如果没有错，就提交事务
  end
 END
+GO</t>
+  </si>
+  <si>
+    <t>USE [PlayNowLog]
+GO
+/****** 对象:  StoredProcedure [dbo].[SP_DownSourceStatistic]    脚本日期: 07/09/2013 15:36:06 ******/
+SET ANSI_NULLS ON
+GO
+SET QUOTED_IDENTIFIER ON
+GO
+-- =============================================
+-- Author:  &lt;Author,,Name&gt;
+-- Create date: &lt;Create Date,,&gt;
+-- Description: 下载来源 分析 包括PlayNow, 百度，其中在做分析插入之前要做一次删除
+-- =============================================
+ALTER PROCEDURE [dbo].[SP_DownSourceStatistic]
+ -- Add the parameters for the stored procedure here
+ @BeginTime Datetime, 
+ @EndTime Datetime
+AS
+BEGIN
+ -- SET NOCOUNT ON added to prevent extra result sets from
+ -- interfering with SELECT statements.
+ SET NOCOUNT ON;
+-- declare @errorCount int=0 --错误的累加
+--2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
+-- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
+declare @errorCount int 
+set @errorCount=0 
+begin  tran --开始事务
+--set @BeginTime=CAST(@BeginTime as date) --开始时间
+--set @EndTime= DATEADD(DD,1, CAST(@EndTime as date)) --结束时间
+set @BeginTime= cast( convert(varchar(10),@BeginTime,120)as datetime)-- CAST(@BeginTime as date) --开始时间
+set @EndTime= cast( convert(varchar(10),DATEADD(DD,1, CAST(@EndTime as datetime)),120)as datetime) --DATEADD(DD,1, CAST(@EndTime as date)) --结束时间
+-- 分析前先删除 某一时间段的数据
+delete from  PN_S_DownSource where CreateTime&gt;=@BeginTime and  CreateTime&lt;@EndTime
+-- PlayNow 下载来源 分析
+insert into PN_S_DownSource(
+  AppName, Publisher, Price, Home, AppDetail, AppRelate,
+  SearchResult, Recommend, RankApp, RankGame, ZoneDetail,
+  CategoryDetail, WapDown,NewApp,NewGame,DownCount, DownCompleteCount, 
+  ContentSource, MachineType, CreateTime
+)
+SELECT  AppName 应用名称,
+  Publisher AS 供应商, 
+  Price AS 单价, 
+  sum(CASE pageName WHEN '首页'     THEN 1 else 0 end) 首页, 
+  sum(CASE pageName WHEN '应用详情'     THEN 1 else 0 end) 应用详情, 
+  sum(CASE pageName WHEN '应用相关'     THEN 1 else 0 end) 应用相关, 
+  sum(CASE pageName WHEN '搜索结果'     THEN 1 else 0 end) 搜索结果, 
+  sum(CASE pageName WHEN '推荐'     THEN 1 else 0 end) 推荐, 
+  sum(CASE pageName WHEN '排行应用'     THEN 1 else 0 end) 排行应用, 
+  sum(CASE pageName WHEN '排行游戏'     THEN 1 else 0 end) 排行游戏, 
+  sum(CASE pageName WHEN '专区详情'     THEN 1 else 0 end) 专区详情, 
+  sum(CASE pageName WHEN '分类详情'     THEN 1 else 0 end) 分类详情, 
+  sum(CASE pageName WHEN 'Wap下载'     THEN 1 else 0 end) Wap下载,
+  sum(CASE pageName WHEN '新品应用'     THEN 1 else 0 end) 新品应用, 
+  sum(CASE pageName WHEN '新品游戏'     THEN 1 else 0 end) 新品游戏, 
+  COUNT(StartTime) as 下载数,
+  sum(CASE  WHEN EndTime is not null   THEN 1 else 0 end) 成功下载数,
+  'PlayNow',
+  MachineType,
+ -- cast(StartTime as date) CreateTime
+ cast( convert(varchar(10),StartTime,120)as datetime) CreateTime
+from dbo.PN_Order 
+WHERE  (IntentFromId !=3 or IntentFromId is null )   
+AND StartTime&gt;= @BeginTime  AND StartTime &lt; @EndTime
+--and  PageName in('首页','应用详情','应用相关','搜索结果','推荐','排行应用','排行游戏',
+--'专区详情','分类详情','Wap下载')
+-- Group by  cast(StartTime as date), MachineType,AppName,Publisher,Price
+ Group by  cast( convert(varchar(10),StartTime,120)as datetime), MachineType,AppName,Publisher,Price
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+--百度下载来源 分析
+insert into PN_S_DownSource(
+  Home, AppRelate,
+  Recommend, RankApp, RankGame, ZoneDetail,
+  CategoryDetail, WapDown, NewApp,NewGame,
+ AppName, Publisher, Price,AppDetail, SearchResult,DownCount,DownCompleteCount,
+ ContentSource,MachineType, CreateTime
+)
+SELECT 
+0,0,0,0,0,0,0,0,0,0,
+  AppName,Publisher,Price,
+  SUM(CASE WHEN pageName='应用详情' THEN 1 ELSE 0 END) 应用详情, 
+  sum(CASE pageName WHEN '搜索结果'     THEN 1 else 0 end) 搜索结果,
+  COUNT(StartTime) as 下载数,
+  sum(CASE  WHEN EndTime is null   THEN 1 else 0 end) 成功下载数,
+  '百度', 
+  MachineType,
+ -- cast(StartTime as date )
+cast( convert(varchar(10),StartTime,120)as datetime)
+from dbo.PN_Order 
+where IntentFromId =3  and  StartTime&gt;=@BeginTime and  StartTime&lt;@EndTime
+and  PageName in('应用详情','搜索结果')
+-- Group by cast(StartTime as date), MachineType,AppName,Publisher,Price
+Group by cast( convert(varchar(10),StartTime,120)as datetime), MachineType,AppName,Publisher,Price
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+if(@errorCount&gt;0)
+ begin
+  rollback --如果有错，就回滚事务
+ end
+else
+ begin
+  commit tran --如果没有错，就提交事务
+ end
+END
+GO</t>
+  </si>
+  <si>
+    <t>USE [PlayNowLog]
+GO
+/****** 对象:  StoredProcedure [dbo].[SP_DeleteStatistic]    脚本日期: 07/09/2013 15:36:06 ******/
+SET ANSI_NULLS ON
+GO
+SET QUOTED_IDENTIFIER ON
+GO
+-- =============================================
+-- Author:  &lt;Author,,Name&gt;
+-- Create date: &lt;Create Date,,&gt;
+-- Description: 删除临时表
+-- =============================================
+ALTER PROCEDURE [dbo].[SP_DeleteStatistic] 
+@BeginTime Datetime, 
+@EndTime Datetime
+AS
+BEGIN
+ -- SET NOCOUNT ON added to prevent extra result sets from
+ -- interfering with SELECT statements.
+ SET NOCOUNT ON;
+--2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
+-- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
+--declare @errorCount int=0 --错误的累加
+declare @errorCount int 
+set @errorCount=0 
+begin  tran --开始事务
+--set @BeginTime=CAST(@BeginTime as date) --开始时间
+--set @EndTime= DATEADD(DD,1, CAST(@EndTime as date)) --结束时间
+set @BeginTime= cast( convert(varchar(10),@BeginTime,120)as datetime) --开始时间
+set @EndTime= cast( convert(varchar(10),DATEADD(DD,1, CAST(@EndTime as datetime)),120)as datetime)--结束时间
+ delete from  dbo.PN_Log_Message where CreateTime&gt;=@BeginTime and CreateTime&lt;@EndTime   --删除消息获取表
+ delete from  dbo.PN_Log_PageViewInfo where DateTime&gt;=@BeginTime and DateTime&lt;@EndTime  --删除PV 日志
+ delete from  dbo.PN_Log_UpdateInfo  where AddTime&gt;=@BeginTime and AddTime&lt;@EndTime --删除升级信息
+ delete from  dbo.PN_Log_SearchKeyword  where CreateTime&gt;=@BeginTime and CreateTime&lt;@EndTime --删除 搜所关键词
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+if(@errorCount&gt;0)
+ begin
+  rollback --如果有错，就回滚事务
+ end
+else
+ begin
+  commit tran --如果没有错，就提交事务
+ end
+END
+GO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE [PlayNowLog]
+GO
+/****** Object:  StoredProcedure [dbo].[SP_DeleteStatistic]    Script Date: 04/24/2013 17:36:58 ******/
+SET ANSI_NULLS ON
+GO
+SET QUOTED_IDENTIFIER ON
+GO
+-- =============================================
+-- Author:  &lt;Author,,Name&gt;
+-- Create date: &lt;Create Date,,&gt;
+-- Description: 删除临时表
+-- =============================================
+alter PROCEDURE [dbo].[SP_DeleteStatistic] 
+@BeginTime Datetime, 
+@EndTime Datetime
+AS
+BEGIN
+ -- SET NOCOUNT ON added to prevent extra result sets from
+ -- interfering with SELECT statements.
+ SET NOCOUNT ON;
+--2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
+-- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
+--declare @errorCount int=0 --错误的累加
+declare @errorCount int 
+set @errorCount=0 
+begin  tran --开始事务
+--set @BeginTime=CAST(@BeginTime as date) --开始时间
+--set @EndTime= DATEADD(DD,1, CAST(@EndTime as date)) --结束时间
+set @BeginTime= cast( convert(varchar(10),@BeginTime,120)as datetime) --开始时间
+set @EndTime= cast( convert(varchar(10),DATEADD(DD,1, CAST(@EndTime as datetime)),120)as datetime)--结束时间
+ delete from  dbo.PN_Log_Message where CreateTime&gt;=@BeginTime and CreateTime&lt;@EndTime   --删除消息获取表
+ delete from  dbo.PN_Log_PageViewInfo where DateTime&gt;=@BeginTime and DateTime&lt;@EndTime  --删除PV 日志
+ delete from  dbo.PN_Log_WebPV where DateTime&gt;=@BeginTime and DateTime&lt;@EndTime  --删除Web-PV 日志
+ delete from  dbo.PN_Log_UpdateInfo  where AddTime&gt;=@BeginTime and AddTime&lt;@EndTime --删除升级信息
+ delete from  dbo.PN_Log_SearchKeyword  where CreateTime&gt;=@BeginTime and CreateTime&lt;@EndTime --删除 搜所关键词
+ --add by rui , delete the temp download data when statistic is done, later could use truncate table
+ -- delete from  dbo.PN_Order  where StartTime&gt;=@BeginTime and StartTime&lt;@EndTime --删除 下载临时数据
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+if(@errorCount&gt;0)
+ begin
+  rollback --如果有错，就回滚事务
+ end
+else
+ begin
+  commit tran --如果没有错，就提交事务
+ end
+END
+GO
 </t>
   </si>
   <si>
-    <t>更新存储过程SP_DownSourceStatistic</t>
-  </si>
-  <si>
-    <t>/****** Object:  StoredProcedure [dbo].[SP_DownSourceStatistic]    Script Date: 04/24/2013 17:36:58 ******/
+    <t>USE [PlayNowLog]
+GO
+/****** Object:  StoredProcedure [dbo].[SP_DownSourceStatistic]    Script Date: 04/24/2013 17:36:58 ******/
 SET ANSI_NULLS ON
 GO
 SET QUOTED_IDENTIFIER ON
@@ -409,59 +864,9 @@
 GO</t>
   </si>
   <si>
-    <t>更新存储过程SP_DeleteStatistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/****** Object:  StoredProcedure [dbo].[SP_DeleteStatistic]    Script Date: 04/24/2013 17:36:58 ******/
-SET ANSI_NULLS ON
-GO
-SET QUOTED_IDENTIFIER ON
-GO
--- =============================================
--- Author:  &lt;Author,,Name&gt;
--- Create date: &lt;Create Date,,&gt;
--- Description: 删除临时表
--- =============================================
-alter PROCEDURE [dbo].[SP_DeleteStatistic] 
-@BeginTime Datetime, 
-@EndTime Datetime
-AS
-BEGIN
- -- SET NOCOUNT ON added to prevent extra result sets from
- -- interfering with SELECT statements.
- SET NOCOUNT ON;
---2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
--- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
---declare @errorCount int=0 --错误的累加
-declare @errorCount int 
-set @errorCount=0 
-begin  tran --开始事务
---set @BeginTime=CAST(@BeginTime as date) --开始时间
---set @EndTime= DATEADD(DD,1, CAST(@EndTime as date)) --结束时间
-set @BeginTime= cast( convert(varchar(10),@BeginTime,120)as datetime) --开始时间
-set @EndTime= cast( convert(varchar(10),DATEADD(DD,1, CAST(@EndTime as datetime)),120)as datetime)--结束时间
- delete from  dbo.PN_Log_Message where CreateTime&gt;=@BeginTime and CreateTime&lt;@EndTime   --删除消息获取表
- delete from  dbo.PN_Log_PageViewInfo where DateTime&gt;=@BeginTime and DateTime&lt;@EndTime  --删除PV 日志
- delete from  dbo.PN_Log_WebPV where DateTime&gt;=@BeginTime and DateTime&lt;@EndTime  --删除Web-PV 日志
- delete from  dbo.PN_Log_UpdateInfo  where AddTime&gt;=@BeginTime and AddTime&lt;@EndTime --删除升级信息
- delete from  dbo.PN_Log_SearchKeyword  where CreateTime&gt;=@BeginTime and CreateTime&lt;@EndTime --删除 搜所关键词
- --add by rui , delete the temp download data when statistic is done, later could use truncate table
- -- delete from  dbo.PN_Order  where StartTime&gt;=@BeginTime and StartTime&lt;@EndTime --删除 下载临时数据
-set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
-if(@errorCount&gt;0)
- begin
-  rollback --如果有错，就回滚事务
- end
-else
- begin
-  commit tran --如果没有错，就提交事务
- end
-END
-GO
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/****** Object:  StoredProcedure [dbo].[SP_DownSourceStatistic]    Script Date: 04/24/2013 17:36:58 ******/
+    <t xml:space="preserve">USE [PlayNowLog]
+GO
+/****** Object:  StoredProcedure [dbo].[SP_DownSourceStatistic]    Script Date: 04/24/2013 17:36:58 ******/
 SET ANSI_NULLS ON
 GO
 SET QUOTED_IDENTIFIER ON
@@ -568,26 +973,7 @@
 </t>
   </si>
   <si>
-    <t>USE [PlayNowLog]
-GO
-/****** Object:  Table [dbo].[PN_S_ExternalAccess]    Script Date: 05/10/2013 10:23:48 ******/
-SET ANSI_NULLS ON
-GO
-SET QUOTED_IDENTIFIER ON
-GO
-CREATE TABLE [dbo].[PN_S_ExternalAccess](
-                [Id] [int] IDENTITY(1,1) NOT NULL,
-                [Name] [nvarchar](200) NULL,
-                [Alias] [nvarchar](200) NULL,
-                [AccessCount] [int] NULL,
-                [CreateTime] [datetime] NULL,
-                [MachineType] [nvarchar](50) NULL,
-CONSTRAINT [PK_PN_ZONE] PRIMARY KEY CLUSTERED 
-(
-                [Id] ASC
-)WITH (PAD_INDEX  = OFF, STATISTICS_NORECOMPUTE  = OFF, IGNORE_DUP_KEY = OFF, ALLOW_ROW_LOCKS  = ON, ALLOW_PAGE_LOCKS  = ON) ON [PRIMARY]
-) ON [PRIMARY]
-GO</t>
+    <t>在表PN_Module上点击右键, 选择打开表，找到‘ModuleName’等于‘页面调用统计’行，然后在表头右键，选择删除</t>
   </si>
   <si>
     <t>USE [PlayNowLog]
@@ -639,109 +1025,100 @@
                 begin
                                 commit tran --如果没有错，就提交事务
                 end
-END</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">修改D:\PlaynowService\AppSettings目录下AppSettings.xml文件：
- 在该文件中
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“&lt;appSettings&gt;”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                后面添加如下内容：
+END
+GO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE [PlayNowLog]
+GO
+/****** Object:  StoredProcedure [dbo].[SP_MessageStatistic]    Script Date: 07/08/2013 11:46:34 ******/
+SET ANSI_NULLS ON
+GO
+SET QUOTED_IDENTIFIER ON
+GO
+-- =============================================
+-- Author:  &lt;Author,,Name&gt;
+-- Create date: &lt;Create Date,,&gt;
+-- Description: 消息统计 分析 其中在做分析插入之前要做一次删除
+-- =============================================
+ALTER PROCEDURE [dbo].[SP_MessageStatistic]
+ -- Add the parameters for the stored procedure here
+ @BeginTime Datetime, 
+ @EndTime Datetime
+AS
+BEGIN
+ -- SET NOCOUNT ON added to prevent extra result sets from
+ -- interfering with SELECT statements.
+ SET NOCOUNT ON;
+--declare @errorCount int=0 --错误的累加
+--2013/4/18 Rui 为了保证向下兼容 sqlserver 2005, 修改此文件 想查看其中变化, 使用文件比较工具与2008脚本进行对比
+-- 变化包括, 变量的定义, 日期的转换 日期类型变为datetime, 并全部转换为零点
+--2013/7/4 jiaoxuhuan ,添加machineType过滤条件。
+declare @errorCount int 
+set @errorCount=0 
+begin  tran --开始事务
+--set @BeginTime=CAST(@BeginTime as date) --开始时间
+--set @EndTime= DATEADD(DD,1, CAST(@EndTime as date)) --结束时间
+set @BeginTime= cast( convert(varchar(10),@BeginTime,120)as datetime) --开始时间
+set @EndTime= cast( convert(varchar(10),DATEADD(DD,1, CAST(@EndTime as datetime)),120)as datetime) --结束时间
+-- 分析前先删除 某一时间段的数据
+delete from  dbo.PN_S_Message where CreateTime&gt;=@BeginTime and  CreateTime&lt;@EndTime
+-- 消息统计 分析
+ insert into dbo.PN_S_Message(
+  MessageID, MachineType, GetMessage,
+  ReadMessage, DownCount,  
+  DownCompleteCount, CreateTime
+ )
+  SELECT  MessageId, MachineType, 
+    (
+    select COUNT(*) from [PN_Log_Message] as A 
+     where C.MessageId=A.MessageId and IsValid=1 and   
+    --CAST(A.CreateTime as date)=cast(C.CreateTime as date) ) as GetCount, 
+    cast( convert(varchar(10),A.CreateTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime)
+    and A.MachineType=C.MachineType
+     ) as GetCount, 
+    (select COUNT(*) from [PN_Log_PageViewInfo] as B 
+    where C.MessageId=B.ContentId AND IntentFromId=4 and
+    -- CAST(B.DateTime as date)=cast(C.CreateTime as date) ) as PVCount,
+    cast( convert(varchar(10),B.DateTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) 
+    and B.MachineType=C.MachineType
+    )as PVCount,
+    (
+    select COUNT(*) from [PN_Order] as D 
+    where C.MessageId=D.ContentId and IntentFromId=4 and
+     --CAST(D.StartTime as date)=cast(C.CreateTime as date) ) as DownCount,
+     cast( convert(varchar(10),D.StartTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime) 
+      and D.MachineType=C.MachineType
+     )as DownCount,
+     (select COUNT(*) from [PN_Order] as G 
+       where C.MessageId=G.ContentId and IntentFromId=4 and
+      -- CAST(G.StartTime as date)=cast(C.CreateTime as date)  
+     cast( convert(varchar(10),G.StartTime,120)as datetime)=cast( convert(varchar(10),C.CreateTime,120)as datetime)
+     and G.MachineType=C.MachineType
+       and EndTime is not null) as DownCompleteCount
+    --,CAST(CreateTime as date) dTime
+    ,cast( convert(varchar(10),CreateTime,120)as datetime) dTime
+  FROM [PN_log_Message] as C
+  where  CreateTime&gt;=@BeginTime AND CreateTime&lt;@EndTime    
+  and MessageId&gt;0 
+  AND IsValid=1 
+  --group by CAST(CreateTime as date),MessageId,MachineType 
+          group by cast( convert(varchar(10),CreateTime,120)as datetime),MessageId,MachineType 
+set @errorCount=@errorCount+@@ERROR --查看是否有错误,做累加
+if(@errorCount&gt;0)
+ begin
+  rollback --如果有错，就回滚事务
+ end
+else
+ begin
+  commit tran --如果没有错，就提交事务
+ end
+END
+GO
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">       &lt;!-- 日志分析器  name：分析器名字， state：分析器状态，on：是可用，off：不可用,
-       platform:平台类型（web/phone/tv）, machineTypes:机器类型，version：客户端版本--&gt;
-  &lt;LogAnalyzers&gt;
-    &lt;LogAnalyzer name="GoogleAnalytics" state="on" platform="phone" machineTypes="" version=""/&gt;
-    &lt;!--&lt;LogAnalyzer name="PlayNowAnalytics" state="off" platform="" machineTypes="" version=""/&gt;--&gt;
-  &lt;/LogAnalyzers&gt;
-</t>
-    </r>
-  </si>
-  <si>
-    <t>更新WebAppStore</t>
-  </si>
-  <si>
-    <t>在windows service中启动playnowlogimport服务</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">修改D:\PlayNowWS_LogImport\WinService目录下PlayNowService.WinServices.exe.config文件：
- 在该文件中
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“&lt;appSettings&gt;”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                后面添加如下内容：
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      &lt;!--download更新每次提交记录数--&gt;
-      &lt;add key="DownloadCommitCount" value="3000" /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>执行如下命令
-cd C:\WINDOWS\Microsoft.NET\Framework\v4.0.30319
-installutil.exe D:\PlayNowWS_LogImport\WinService\PlayNowService.WinService.Log.exe</t>
-  </si>
-  <si>
-    <t>备份10.126.64.14（115.182.57.20）服务器下的D:\WebAppStore目录</t>
-  </si>
-  <si>
-    <t>删除D:\WebAppStore目录下除Web.config的所有文件</t>
+  </si>
+  <si>
+    <t>删除D:\PlaynowService目录下除Log、AppSettings和Web.config的所有文件</t>
   </si>
   <si>
     <t>USE [PlayNowLog]
@@ -856,34 +1233,11 @@
  begin
   commit tran --如果没有错，就提交事务
  end
-END</t>
-  </si>
-  <si>
-    <t>删除D:\PlayNowManage目录下除Web.config的所有文件</t>
-  </si>
-  <si>
-    <t>所有安装包所在文件夹为v5.4.130716\Deploy Packages\PlayNowService</t>
-  </si>
-  <si>
-    <t>复制文件夹v5.4.130716\Deploy Packages\PlayNowService下的全部文件到D:\PlaynowService目录</t>
-  </si>
-  <si>
-    <t>所有安装包所在文件夹为v5.4.130716\Deploy Packages\WinService</t>
-  </si>
-  <si>
-    <t>将更新文件夹v5.4.130716\Deploy Packages\WinService下的内容拷贝到D:\PlayNowWS_LogImport\WinService目录下</t>
-  </si>
-  <si>
-    <t>所有安装包所在文件夹为 v5.4.130716\Deploy Packages\PlayNowManager</t>
-  </si>
-  <si>
-    <t>复制文件夹 v5.4.130716\Deploy Packages\PlayNowManager下的全部文件到D:\PlayNowManage 目录</t>
-  </si>
-  <si>
-    <t>所有安装包所在文件夹为  v5.4.130716\Deploy Packages\WebAppStore</t>
-  </si>
-  <si>
-    <t>复制文件夹v5.4.130716\Deploy Packages\WebAppStore下的全部文件到D:\WebAppStore目录</t>
+END
+GO</t>
+  </si>
+  <si>
+    <t>备份10.126.64.18（10.126.64.19）服务器下的D:\WebAppStore目录</t>
   </si>
 </sst>
 </file>
@@ -963,7 +1317,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1161,9 +1514,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1172,6 +1522,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1515,7 +1868,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -1523,7 +1876,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -1531,7 +1884,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:3">
@@ -1539,7 +1892,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1552,8 +1905,8 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1591,13 +1944,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75.75" customHeight="1">
@@ -1607,13 +1960,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>22</v>
+      <c r="F3" s="23" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="52.5" customHeight="1">
@@ -1623,31 +1976,31 @@
         <v>3</v>
       </c>
       <c r="D4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="21">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="69" customHeight="1">
@@ -1657,13 +2010,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="73.5" customHeight="1">
@@ -1673,13 +2026,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="72" customHeight="1">
@@ -1689,13 +2042,13 @@
         <v>4</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>55</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="70.5" customHeight="1">
@@ -1705,13 +2058,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="78" customHeight="1">
@@ -1720,62 +2073,62 @@
       <c r="C10" s="7">
         <v>7</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>39</v>
+      <c r="D10" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>38</v>
+        <v>64</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="78" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="27"/>
-      <c r="C11" s="23">
+      <c r="C11" s="22">
         <v>8</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>41</v>
+      <c r="D11" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>38</v>
+        <v>60</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="73.5" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="27"/>
-      <c r="C12" s="23">
+      <c r="C12" s="22">
         <v>9</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>43</v>
+      <c r="D12" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>38</v>
+        <v>59</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="73.5" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="23">
+      <c r="C13" s="22">
         <v>10</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>41</v>
+      <c r="D13" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>38</v>
+        <v>61</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +2147,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1805,7 +2158,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="28" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1830,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="165">
@@ -1838,7 +2191,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1846,7 +2199,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1870,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1882,7 +2235,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="28" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1923,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" ht="90">
@@ -1931,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -1940,7 +2293,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1948,7 +2301,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1978,7 +2331,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="28" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1997,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1">
@@ -2005,7 +2358,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2028,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2040,7 +2393,7 @@
     <row r="1" spans="1:2">
       <c r="A1" s="10"/>
       <c r="B1" s="28" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2052,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2060,7 +2413,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -2068,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2085,4 +2438,145 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all/>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type" ma:readOnly="true"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="3" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{682123CB-425B-4A64-BDB0-F7245F839F73}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D297F45-1728-49FB-AC2E-7F3D4B19A3E0}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A814B3F-BD5D-4C29-A2D1-8AD02E9CC0E5}"/>
 </file>
</xml_diff>